<commit_message>
Enhance Excel export functionality and add new imports for openpyxl styles
</commit_message>
<xml_diff>
--- a/课程表.xlsx
+++ b/课程表.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="课程表" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,17 +27,33 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="16"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCCCCC"/>
+        <bgColor rgb="00CCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffcccc"/>
+        <bgColor rgb="00ffcccc"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,41 +61,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,130 +441,92 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>地点</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>教师</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>课程名称</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="n"/>
+    <row r="1" ht="60" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>课程表</t>
+        </is>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>星期</t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>周一</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>周四</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>周一</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>周四</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>周一</t>
-        </is>
-      </c>
-      <c r="G2" s="1" t="inlineStr">
-        <is>
-          <t>周四</t>
+    <row r="2" ht="60" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>节次</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>星期一</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>星期二</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>星期三</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>星期四</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>星期五</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>星期六</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>星期日</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>节次</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="3" ht="60" customHeight="1">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>教室</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>周周</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>语文</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>未指定</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>王老师</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>数学</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:E1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>